<commit_message>
Change status of episode 1 to 5
Signed-off-by: Stefan Kühnel <git@stefankuehnel.com>
</commit_message>
<xml_diff>
--- a/collection.xlsx
+++ b/collection.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conta\Desktop\naruto-shippuden.datasette.stefan-dev.de\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conta\Desktop\naruto.dvd.stefan-dev.de\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -560,7 +560,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,7 +588,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -599,7 +599,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -610,7 +610,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -621,7 +621,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -632,7 +632,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>